<commit_message>
Added context menu, bookmarks, interactivity-service. Upgraded API to v2.3.0
</commit_message>
<xml_diff>
--- a/documents/Published/Quadrant Chart/QuadrantChartByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Quadrant Chart/QuadrantChartByMAQSoftwareChecklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CustomVisuals\documents\Published\Quadrant Chart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAQUser\source\repos\NewRepo2\documents\Published\Quadrant Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F36A8E-609C-4C18-B497-E80BB73AED41}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA03EB3-53FD-403C-9858-80E37D718505}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24360" windowHeight="9240" xr2:uid="{E6ADFF9B-929E-442F-838C-1C0C2035D4F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6ADFF9B-929E-442F-838C-1C0C2035D4F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="83">
   <si>
     <t>S no</t>
   </si>
@@ -266,15 +266,26 @@
     <t>Save selections &amp; filtering in a bookmark</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>3. In the Bookmarks Pane, add a new bookmark and 'update' it</t>
   </si>
   <si>
     <t>1. Bookmarks Pane will be visible on the right side
 2. A new bookmark entry will be added in the pane
 3. Previously saved state will be rendered in the visual with saved selections and filtering</t>
+  </si>
+  <si>
+    <t>Drillthrough</t>
+  </si>
+  <si>
+    <t>Created custom menu to drill through from one visual to another.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Generate a chart with some data
+2.Create new report page and in DrillThrough add the fields for drillthrough.
+3. Right click on the chart, select the Drillthrough option from the menu. </t>
+  </si>
+  <si>
+    <t>1. On right click of the chart and selecting the drillthrough option from the context-menu , the report will drillthrough to the newly created report page.</t>
   </si>
 </sst>
 </file>
@@ -321,7 +332,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -329,11 +340,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -350,20 +370,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -372,16 +389,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -389,8 +406,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -706,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3542ACED-FC5A-41CE-B411-3B15EAE34D58}">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:A60"/>
+      <selection activeCell="B4" sqref="B4:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,22 +740,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>45</v>
       </c>
       <c r="G1" s="9"/>
@@ -746,49 +763,49 @@
       <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="12" t="s">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+      <c r="A4" s="13">
         <v>1</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="12" t="s">
         <v>68</v>
       </c>
       <c r="F4" s="9" t="s">
@@ -805,41 +822,41 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="8" t="s">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="15"/>
+      <c r="E5" s="12"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="8" t="s">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="15"/>
+      <c r="E6" s="12"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="10" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="9" t="s">
@@ -856,45 +873,45 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="10"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="15"/>
+      <c r="E8" s="12"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="10"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="15"/>
+      <c r="E9" s="12"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="A10" s="13">
         <v>2</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="14" t="s">
         <v>43</v>
       </c>
       <c r="F10" s="9" t="s">
@@ -911,41 +928,41 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="13"/>
+      <c r="E11" s="14"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
     </row>
     <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="13"/>
+      <c r="E12" s="14"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="10" t="s">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="13" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="12" t="s">
         <v>52</v>
       </c>
       <c r="F13" s="9" t="s">
@@ -962,41 +979,41 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="10"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="13"/>
+      <c r="E14" s="14"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="10"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="13"/>
       <c r="D15" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="13"/>
+      <c r="E15" s="14"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="10" t="s">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="13" t="s">
         <v>16</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="14" t="s">
         <v>18</v>
       </c>
       <c r="F16" s="9" t="s">
@@ -1013,45 +1030,45 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="10"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="13"/>
       <c r="D17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="13"/>
+      <c r="E17" s="14"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="10"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="13"/>
       <c r="D18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="13"/>
+      <c r="E18" s="14"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
+      <c r="A19" s="13">
         <v>3</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="13" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="12" t="s">
         <v>54</v>
       </c>
       <c r="F19" s="9" t="s">
@@ -1068,54 +1085,54 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
       <c r="D20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="13"/>
+      <c r="E20" s="14"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
       <c r="D21" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="13"/>
+      <c r="E21" s="14"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
       <c r="D22" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="13"/>
+      <c r="E22" s="14"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="10" t="s">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="13" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="14" t="s">
         <v>42</v>
       </c>
       <c r="F23" s="9" t="s">
@@ -1132,41 +1149,41 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="10"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="13"/>
       <c r="D24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="13"/>
+      <c r="E24" s="14"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="10"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="13"/>
       <c r="D25" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="13"/>
+      <c r="E25" s="14"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="10" t="s">
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="13" t="s">
         <v>25</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="E26" s="12" t="s">
         <v>69</v>
       </c>
       <c r="F26" s="9" t="s">
@@ -1183,71 +1200,71 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="10"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="13"/>
       <c r="D27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="15"/>
+      <c r="E27" s="12"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="10"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="13"/>
       <c r="D28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="15"/>
+      <c r="E28" s="12"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="7" t="s">
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="15"/>
+      <c r="E29" s="12"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="10"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="13"/>
       <c r="D30" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E30" s="15"/>
+      <c r="E30" s="12"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="10">
+      <c r="A31" s="13">
         <v>4</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="13" t="s">
         <v>29</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="E31" s="14" t="s">
         <v>31</v>
       </c>
       <c r="F31" s="9" t="s">
@@ -1264,54 +1281,54 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
       <c r="D32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E32" s="13"/>
+      <c r="E32" s="14"/>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
       <c r="D33" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E33" s="13"/>
+      <c r="E33" s="14"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
       <c r="D34" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E34" s="13"/>
+      <c r="E34" s="14"/>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
       <c r="I34" s="9"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="10" t="s">
+      <c r="A35" s="15"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="13" t="s">
         <v>32</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="12" t="s">
         <v>44</v>
       </c>
       <c r="F35" s="9" t="s">
@@ -1328,41 +1345,41 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="10"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="13"/>
       <c r="D36" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E36" s="13"/>
+      <c r="E36" s="14"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
       <c r="I36" s="9"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="10"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="13"/>
       <c r="D37" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E37" s="13"/>
+      <c r="E37" s="14"/>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
       <c r="I37" s="9"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="10" t="s">
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="13" t="s">
         <v>33</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="E38" s="12" t="s">
         <v>69</v>
       </c>
       <c r="F38" s="9" t="s">
@@ -1379,71 +1396,71 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="10"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="13"/>
       <c r="D39" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E39" s="15"/>
+      <c r="E39" s="12"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
       <c r="I39" s="9"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="10"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="13"/>
       <c r="D40" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="15"/>
+      <c r="E40" s="12"/>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
       <c r="I40" s="9"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="7" t="s">
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E41" s="15"/>
+      <c r="E41" s="12"/>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="10"/>
+      <c r="A42" s="15"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="13"/>
       <c r="D42" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E42" s="15"/>
+      <c r="E42" s="12"/>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="10">
+      <c r="A43" s="13">
         <v>5</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="13" t="s">
         <v>35</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="E43" s="12" t="s">
         <v>70</v>
       </c>
       <c r="F43" s="9" t="s">
@@ -1460,71 +1477,71 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
       <c r="D44" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E44" s="15"/>
+      <c r="E44" s="12"/>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
       <c r="H44" s="9"/>
       <c r="I44" s="9"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="10"/>
-      <c r="B45" s="10"/>
-      <c r="C45" s="10"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
       <c r="D45" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E45" s="15"/>
+      <c r="E45" s="12"/>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
       <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="10"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
       <c r="D46" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E46" s="15"/>
+      <c r="E46" s="12"/>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
       <c r="H46" s="9"/>
       <c r="I46" s="9"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="10"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
       <c r="D47" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E47" s="15"/>
+      <c r="E47" s="12"/>
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
       <c r="I47" s="9"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="10">
+      <c r="A48" s="13">
         <v>6</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="C48" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D48" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E48" s="15" t="s">
+      <c r="E48" s="12" t="s">
         <v>61</v>
       </c>
       <c r="F48" s="9" t="s">
@@ -1541,54 +1558,54 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="10"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="6" t="s">
+      <c r="A49" s="13"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E49" s="15"/>
+      <c r="E49" s="12"/>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
       <c r="H49" s="9"/>
       <c r="I49" s="9"/>
     </row>
     <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="6" t="s">
+      <c r="A50" s="13"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E50" s="15"/>
+      <c r="E50" s="12"/>
       <c r="F50" s="9"/>
       <c r="G50" s="9"/>
       <c r="H50" s="9"/>
       <c r="I50" s="9"/>
     </row>
     <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="6" t="s">
+      <c r="A51" s="13"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E51" s="15"/>
+      <c r="E51" s="12"/>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
       <c r="I51" s="9"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="16" t="s">
+      <c r="A52" s="13"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="D52" s="6" t="s">
+      <c r="D52" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E52" s="15" t="s">
+      <c r="E52" s="12" t="s">
         <v>61</v>
       </c>
       <c r="F52" s="9" t="s">
@@ -1605,127 +1622,160 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="10"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="6" t="s">
+      <c r="A53" s="13"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E53" s="15"/>
+      <c r="E53" s="12"/>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
       <c r="H53" s="9"/>
       <c r="I53" s="9"/>
     </row>
     <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="10"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="6" t="s">
+      <c r="A54" s="13"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E54" s="15"/>
+      <c r="E54" s="12"/>
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
       <c r="H54" s="9"/>
       <c r="I54" s="9"/>
     </row>
     <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="10"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="6" t="s">
+      <c r="A55" s="13"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E55" s="15"/>
+      <c r="E55" s="12"/>
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
       <c r="I55" s="9"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="14">
+      <c r="A56" s="15">
         <v>7</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C56" s="14" t="s">
+      <c r="C56" s="15" t="s">
         <v>76</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E56" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="F56" s="19" t="s">
+      <c r="E56" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F56" s="9" t="s">
         <v>50</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="H56" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="I56" s="19" t="s">
-        <v>77</v>
+        <v>50</v>
+      </c>
+      <c r="I56" s="9" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
+      <c r="A57" s="15"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
       <c r="D57" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E57" s="18"/>
-      <c r="F57" s="19"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="9"/>
       <c r="G57" s="9"/>
       <c r="H57" s="9"/>
-      <c r="I57" s="19"/>
+      <c r="I57" s="9"/>
     </row>
     <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
+      <c r="A58" s="15"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="15"/>
       <c r="D58" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E58" s="18"/>
-      <c r="F58" s="19"/>
+        <v>77</v>
+      </c>
+      <c r="E58" s="17"/>
+      <c r="F58" s="9"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
-      <c r="I58" s="19"/>
+      <c r="I58" s="9"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
+      <c r="A59" s="15"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="15"/>
       <c r="D59" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E59" s="18"/>
-      <c r="F59" s="19"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="9"/>
       <c r="G59" s="9"/>
       <c r="H59" s="9"/>
-      <c r="I59" s="19"/>
+      <c r="I59" s="9"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
+      <c r="A60" s="15"/>
+      <c r="B60" s="15"/>
+      <c r="C60" s="15"/>
       <c r="D60" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E60" s="18"/>
-      <c r="F60" s="19"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="9"/>
       <c r="G60" s="9"/>
       <c r="H60" s="9"/>
-      <c r="I60" s="19"/>
+      <c r="I60" s="9"/>
+    </row>
+    <row r="61" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>8</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H61" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I61" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="128">
+    <mergeCell ref="F52:F55"/>
+    <mergeCell ref="G52:G55"/>
+    <mergeCell ref="H52:H55"/>
+    <mergeCell ref="I52:I55"/>
     <mergeCell ref="E56:E60"/>
     <mergeCell ref="B56:B60"/>
     <mergeCell ref="C56:C60"/>
@@ -1734,6 +1784,19 @@
     <mergeCell ref="G56:G60"/>
     <mergeCell ref="H56:H60"/>
     <mergeCell ref="I56:I60"/>
+    <mergeCell ref="B48:B55"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="E26:E30"/>
+    <mergeCell ref="I43:I47"/>
+    <mergeCell ref="F48:F51"/>
+    <mergeCell ref="G48:G51"/>
+    <mergeCell ref="H48:H51"/>
+    <mergeCell ref="I48:I51"/>
     <mergeCell ref="F35:F37"/>
     <mergeCell ref="G35:G37"/>
     <mergeCell ref="H35:H37"/>
@@ -1743,22 +1806,13 @@
     <mergeCell ref="H38:H42"/>
     <mergeCell ref="I38:I42"/>
     <mergeCell ref="C48:C51"/>
-    <mergeCell ref="B48:B55"/>
-    <mergeCell ref="C52:C55"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="E52:E55"/>
     <mergeCell ref="F43:F47"/>
     <mergeCell ref="G43:G47"/>
     <mergeCell ref="H43:H47"/>
-    <mergeCell ref="I43:I47"/>
-    <mergeCell ref="F48:F51"/>
-    <mergeCell ref="G48:G51"/>
-    <mergeCell ref="H48:H51"/>
-    <mergeCell ref="I48:I51"/>
-    <mergeCell ref="F52:F55"/>
-    <mergeCell ref="G52:G55"/>
-    <mergeCell ref="H52:H55"/>
-    <mergeCell ref="I52:I55"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="E16:E18"/>
     <mergeCell ref="E43:E47"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B7:B9"/>
@@ -1768,6 +1822,26 @@
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="E10:E12"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="C38:C42"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="C26:C30"/>
+    <mergeCell ref="E38:E42"/>
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="B43:B47"/>
+    <mergeCell ref="C43:C47"/>
+    <mergeCell ref="A48:A55"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="A1:A3"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:C6"/>
@@ -1783,35 +1857,15 @@
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="C13:C15"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="C38:C42"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="C26:C30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="E26:E30"/>
-    <mergeCell ref="E38:E42"/>
-    <mergeCell ref="A43:A47"/>
-    <mergeCell ref="B43:B47"/>
-    <mergeCell ref="C43:C47"/>
-    <mergeCell ref="A48:A55"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="G16:G18"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="I16:I18"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
@@ -1821,15 +1875,7 @@
     <mergeCell ref="G4:G6"/>
     <mergeCell ref="H4:H6"/>
     <mergeCell ref="I4:I6"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="G16:G18"/>
-    <mergeCell ref="H16:H18"/>
-    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="E13:E15"/>
     <mergeCell ref="F19:F22"/>
     <mergeCell ref="G19:G22"/>
     <mergeCell ref="H19:H22"/>

</xml_diff>